<commit_message>
Sat Jan 25 01:48:20 PM EST 2025
</commit_message>
<xml_diff>
--- a/ozone/ozone_MB_SHAP.xlsx
+++ b/ozone/ozone_MB_SHAP.xlsx
@@ -447,548 +447,548 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(h$_{rs}$)$_{2}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0005002810669310267</v>
+        <v>0.0007884131613055202</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>h$_{q}$</t>
+          <t>type_3</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0003338417503463099</v>
+        <v>0.000322927768047953</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(h$_{r}$)$_{3}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0002427856377536234</v>
+        <v>0.0003067387437633452</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0002250269100608179</v>
+        <v>0.0002975048811480967</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
+          <t>(h$_{rs}$)$_{2}$</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.0001749420041476334</v>
+        <v>0.0002664597228640155</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>7</v>
+        <v>100</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{3}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.0001621408418555507</v>
+        <v>0.0002662795993532965</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
+          <t>h$_{q}$</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0001541894049539742</v>
+        <v>0.0002576803311019357</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>type_3</t>
+          <t>(h$_{p}$)$_{0}$</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.0001461465366119957</v>
+        <v>0.0001856690913506954</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{2}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0001380046336020249</v>
+        <v>0.0001133441682635461</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{3}$</t>
+          <t>(h$_{pq}$)$_{3}$</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0001211622703530315</v>
+        <v>0.0001024653146636197</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>101</v>
+        <v>2</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
+          <t>(h$_{p}$)$_{2}$</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0001126580569157614</v>
+        <v>0.0001022578400752484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>$F_{s}$</t>
+          <t>(h$_{p}$)$_{3}$</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.0001054171918358657</v>
+        <v>9.554433279633899e-05</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
+          <t>$\eta_{s}$</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8.686007903918304e-05</v>
+        <v>9.417398523579203e-05</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{2}$</t>
+          <t>(h$_{pq}$)$_{2}$</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8.562787623638355e-05</v>
+        <v>8.716705476203208e-05</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>h$_{s}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>8.485794365801569e-05</v>
+        <v>8.43844134966694e-05</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>8.245151223061883e-05</v>
+        <v>8.357099598998129e-05</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>(h$_{p}$)$_{3}$</t>
+          <t>(h$_{rs}$)$_{3}$</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>7.906611158703412e-05</v>
+        <v>7.984183706469344e-05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{2}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>6.792384509299642e-05</v>
+        <v>7.073524816935775e-05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>(h$_{rs}$)$_{3}$</t>
+          <t>$F_{q}^{\text{SCF}}$</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6.359025892607381e-05</v>
+        <v>6.170336761249203e-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>h$_{qs}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6.310987498082204e-05</v>
+        <v>5.516518724836384e-05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>(h$_{p}$)$_{0}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>6.30829954833777e-05</v>
+        <v>5.369678198097799e-05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{0}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.168972724619051e-05</v>
+        <v>4.849767586844507e-05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{2}$</t>
+          <t>$F_{s}^{\text{SCF}}$</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>6.048681232893712e-05</v>
+        <v>4.736710477019953e-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{3}$</t>
+          <t>(h$_{r}$)$_{3}$</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>5.345578826812939e-05</v>
+        <v>4.695099740735827e-05</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>(h$_{r}$)$_{2}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4.966117244357857e-05</v>
+        <v>4.639707945542679e-05</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert qp \rangle)_{1}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4.220244800009391e-05</v>
+        <v>4.048390113164428e-05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>(h$_{p}$)$_{1}$</t>
+          <t>(h$_{r}$)$_{2}$</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>4.158743726761654e-05</v>
+        <v>3.985884519248083e-05</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{3}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>4.134621442931277e-05</v>
+        <v>3.867932734174707e-05</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>(h$_{r}$)$_{1}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3.657812526087462e-05</v>
+        <v>3.724854114468233e-05</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{0}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>3.568398815032549e-05</v>
+        <v>3.580848053342746e-05</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
+          <t>$(\eta_{r})_{0}$</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3.486036249361397e-05</v>
+        <v>3.53627564107335e-05</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>$F_{s}^{\text{SCF}}$</t>
+          <t>$\langle qq \vert qq \rangle$</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3.481574029411694e-05</v>
+        <v>3.26920190119951e-05</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{3}$</t>
+          <t>(h$_{p}$)$_{1}$</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>3.249811188861491e-05</v>
+        <v>3.0790636671121e-05</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{1}$</t>
+          <t>$(\langle rs \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3.121550850384764e-05</v>
+        <v>2.955583441443358e-05</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>$F_{q}^{\text{SCF}}$</t>
+          <t>(h$_{pq}$)$_{0}$</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2.894080862325967e-05</v>
+        <v>2.570828771925061e-05</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{1}$</t>
+          <t>(h$_{r}$)$_{1}$</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2.362786758361246e-05</v>
+        <v>2.457893716736419e-05</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>(h$_{p}$)$_{2}$</t>
+          <t>h$_{qs}$</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2.199069321622951e-05</v>
+        <v>2.271365358166182e-05</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
+          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2.027495009346288e-05</v>
+        <v>2.269106172574525e-05</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert pq \rangle)_{0}$</t>
+          <t>$\langle ss \vert ss \rangle$</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1.937754991253403e-05</v>
+        <v>2.136113123512338e-05</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>(h$_{pr}$)$_{1}$</t>
+          <t>h$_{s}$</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1.881283731039587e-05</v>
+        <v>1.931270650902697e-05</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>$(\langle rs \vert sr \rangle)_{1}$</t>
+          <t>$F_{q}$</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1.748475530700164e-05</v>
+        <v>1.899315261014967e-05</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>$F_{q}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.571693657567825e-05</v>
+        <v>1.766315758194122e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1001,553 +1001,553 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.491849212066641e-05</v>
+        <v>1.617678414818546e-05</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>76</v>
+        <v>11</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
+          <t>(h$_{pr}$)$_{3}$</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.413567960554109e-05</v>
+        <v>1.551662777237981e-05</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{1}$</t>
+          <t>$(\langle pq \vert qp \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.405912022870994e-05</v>
+        <v>1.489327647034565e-05</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1.1868427176169e-05</v>
+        <v>1.36724593509816e-05</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>$\langle ss \vert ss \rangle$</t>
+          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.130892566784679e-05</v>
+        <v>1.208447585502166e-05</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>11</v>
+        <v>88</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>(h$_{pr}$)$_{3}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.127709813605188e-05</v>
+        <v>1.182116207606945e-05</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>$\eta_{s}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.058264818333883e-05</v>
+        <v>1.180556961443771e-05</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>9.156432215233495e-06</v>
+        <v>1.155273589511655e-05</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>(h$_{pr}$)$_{2}$</t>
+          <t>$(F_{r})_{0}$</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7.345937578047545e-06</v>
+        <v>1.129953846558864e-05</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{2}$</t>
+          <t>(h$_{r}$)$_{0}$</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>7.010802070446913e-06</v>
+        <v>1.128651924249627e-05</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>$\langle qq \vert qq \rangle$</t>
+          <t>$(\langle rs \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>6.034821110475783e-06</v>
+        <v>1.066988647551382e-05</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{0}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>5.867489987995058e-06</v>
+        <v>9.86155877411778e-06</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
+          <t>$(F_{r})_{1}$</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5.802836708918853e-06</v>
+        <v>9.799594566787598e-06</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{0}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>5.47828021004755e-06</v>
+        <v>9.434062764478771e-06</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{1}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>4.97024746053688e-06</v>
+        <v>7.908487872212489e-06</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>(h$_{rs}$)$_{1}$</t>
+          <t>(h$_{rs}$)$_{0}$</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>4.74980635531991e-06</v>
+        <v>6.862071721934525e-06</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>$(F_{r})_{1}$</t>
+          <t>type_2</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>4.693425497596242e-06</v>
+        <v>6.725403039604658e-06</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{3}$</t>
+          <t>(h$_{pq}$)$_{1}$</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>4.591099000046427e-06</v>
+        <v>6.545269859355761e-06</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{0}$</t>
+          <t>$F_{s}$</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>4.195565499304376e-06</v>
+        <v>6.444130238370042e-06</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>type_1</t>
+          <t>(h$_{rs}$)$_{1}$</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>3.833683969863022e-06</v>
+        <v>5.364042622435498e-06</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{0}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>3.796231898096392e-06</v>
+        <v>5.222559050844793e-06</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>3.760855686559675e-06</v>
+        <v>5.104094825522702e-06</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>(h$_{rs}$)$_{0}$</t>
+          <t>(h$_{pr}$)$_{1}$</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>3.615192708841224e-06</v>
+        <v>4.930682787194932e-06</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>(h$_{r}$)$_{0}$</t>
+          <t>(h$_{pr}$)$_{0}$</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2.738555598709936e-06</v>
+        <v>4.383638410475236e-06</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2.479100141120424e-06</v>
+        <v>3.665273751117964e-06</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>type_0</t>
+          <t>$(\eta_{p})_{2}$</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>2.216848194297511e-06</v>
+        <v>3.612062657585257e-06</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>$(F_{r})_{0}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2.004014752041688e-06</v>
+        <v>3.535822804642565e-06</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{2}$</t>
+          <t>$(\eta_{p})_{1}$</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1.441955806542966e-06</v>
+        <v>3.148302186401082e-06</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
+          <t>$(\eta_{p})_{3}$</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>8.350428310069741e-07</v>
+        <v>2.757825678971191e-06</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{3}$</t>
+          <t>(h$_{pr}$)$_{2}$</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>3.306957632833059e-07</v>
+        <v>2.611335065194781e-06</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>$(F_{p})_{0}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{1}$</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>2.443418583852123e-07</v>
+        <v>2.561044959328004e-06</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>81</v>
+        <v>24</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{1}$</t>
+          <t>type_1</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1.74497926025138e-07</v>
+        <v>2.105086285516744e-06</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
+          <t>$(\eta_{r})_{3}$</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2.699659364055101e-08</v>
+        <v>1.992730612473577e-06</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>$(F_{p})_{1}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2.5391419815371e-08</v>
+        <v>9.909953475972007e-07</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>type_2</t>
+          <t>$(\eta_{r})_{1}$</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2.009697541890371e-08</v>
+        <v>6.415672878599415e-07</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{0}$</t>
+          <t>$(\omega_{r})_{3}$</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1.959924336880241e-08</v>
+        <v>3.10225691966246e-07</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
+          <t>$(F_{p})_{1}$</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1.930541201820953e-08</v>
+        <v>1.976213927480166e-07</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>(h$_{pr}$)$_{0}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1.57045588011799e-08</v>
+        <v>2.08113804388708e-08</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{1}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1.387066904900376e-08</v>
+        <v>1.868466717638319e-08</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1.3415067771343e-08</v>
+        <v>1.518086323351555e-08</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{1}$</t>
+          <t>$(\omega_{r})_{2}$</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1.302458122248416e-08</v>
+        <v>1.515343514704689e-08</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{1}$</t>
+          <t>type_0</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1.260215768284816e-08</v>
+        <v>1.484411868461944e-08</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>$(\eta_{r})_{2}$</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1.145722053064836e-08</v>
+        <v>1.105561724229578e-08</v>
       </c>
     </row>
     <row r="87">
@@ -1560,137 +1560,137 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>1.095009789265479e-08</v>
+        <v>8.290092396698317e-09</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>$(F_{p})_{2}$</t>
+          <t>$(F_{p})_{0}$</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1.065061581770802e-08</v>
+        <v>7.18241115438126e-09</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
+          <t>$(F_{r})_{2}$</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>9.762021730171498e-09</v>
+        <v>6.828735153894927e-09</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{0}$</t>
+          <t>$(F_{p})_{2}$</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>9.267208246871647e-09</v>
+        <v>6.193047527736707e-09</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{2}$</t>
+          <t>$(\eta_{p})_{0}$</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>9.092735402315246e-09</v>
+        <v>4.619573345458474e-09</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>$\mathbf{b}$</t>
+          <t>$(\omega_{p})_{0}$</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>8.361258885174856e-09</v>
+        <v>4.616293628477568e-09</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$(F_{r})_{2}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>8.341288939813728e-09</v>
+        <v>3.25232924412816e-09</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$(F_{p})_{3}$</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>8.314874215788606e-09</v>
+        <v>3.227698866596772e-09</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>$(F_{p})_{3}$</t>
+          <t>$(\omega_{r})_{0}$</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>6.765276038795064e-09</v>
+        <v>3.125201963985733e-09</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{2}$</t>
+          <t>$(\omega_{p})_{1}$</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>4.822657178905268e-09</v>
+        <v>2.965430462938812e-09</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{2}$</t>
+          <t>$\mathbf{b}$</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>4.49799716775282e-09</v>
+        <v>1.18838234165969e-09</v>
       </c>
     </row>
     <row r="98">
@@ -1703,7 +1703,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>3.512372984863087e-09</v>
+        <v>1.120235749007456e-09</v>
       </c>
     </row>
     <row r="99">
@@ -1716,55 +1716,55 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>2.825079834979144e-09</v>
+        <v>5.588863395910018e-10</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{0}$</t>
+          <t>$\omega_{s}$</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>2.476519491837379e-09</v>
+        <v>5.443392750010538e-10</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{3}$</t>
+          <t>$(\omega_{p})_{2}$</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>2.078725893156511e-09</v>
+        <v>1.449947363205186e-10</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>$\omega_{s}$</t>
+          <t>$\omega_{q}$</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1.970109593886829e-09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>$\omega_{q}$</t>
+          <t>$(\omega_{p})_{3}$</t>
         </is>
       </c>
       <c r="C103" t="n">

</xml_diff>

<commit_message>
Mon Jan 27 10:05:17 PM EST 2025 update figures for manuscript
</commit_message>
<xml_diff>
--- a/ozone/ozone_MB_SHAP.xlsx
+++ b/ozone/ozone_MB_SHAP.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0008885679624585211</v>
+        <v>0.0008892826004847061</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0006816368138988936</v>
+        <v>0.000678641705020092</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0004213287417544945</v>
+        <v>0.0004185367885651768</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0003724065203832983</v>
+        <v>0.0003770353426672187</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.000314284507518904</v>
+        <v>0.000318408844430717</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.0002863027837880087</v>
+        <v>0.000282804012915769</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0002622142248995958</v>
+        <v>0.0002649591332523719</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.0001827370101012143</v>
+        <v>0.0001743158079944655</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0001609187859808239</v>
+        <v>0.0001603683158761672</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0001190145357233996</v>
+        <v>0.0001187498436718664</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0001119295962487184</v>
+        <v>0.0001179385892459306</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.0001080358736867315</v>
+        <v>0.000106636775606351</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9.166098506822979e-05</v>
+        <v>9.139713873590455e-05</v>
       </c>
     </row>
     <row r="15">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8.545055940249606e-05</v>
+        <v>8.581071873985629e-05</v>
       </c>
     </row>
     <row r="16">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>7.922180037418157e-05</v>
+        <v>7.984438912437895e-05</v>
       </c>
     </row>
     <row r="17">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6.862860336921204e-05</v>
+        <v>6.75965346257002e-05</v>
       </c>
     </row>
     <row r="18">
@@ -663,85 +663,85 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>6.599879746139045e-05</v>
+        <v>6.51821297973602e-05</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>$F_{q}^{\text{SCF}}$</t>
+          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>6.564996178247912e-05</v>
+        <v>6.089659296894452e-05</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>92</v>
+        <v>21</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>$(\langle rs\vert rs \rangle)_{2}$</t>
+          <t>(h$_{rs}$)$_{3}$</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6.147042345129935e-05</v>
+        <v>6.082314601596453e-05</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>(h$_{rs}$)$_{3}$</t>
+          <t>$F_{q}^{\text{SCF}}$</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6.096952341103291e-05</v>
+        <v>6.038503571868398e-05</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{0}$</t>
+          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4.824431864839864e-05</v>
+        <v>4.914754399614944e-05</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>$(F_{p}^{\text{SCF}})_{2}$</t>
+          <t>(h$_{pq}$)$_{2}$</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4.680148574669006e-05</v>
+        <v>4.638017750896637e-05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{2}$</t>
+          <t>(h$_{pq}$)$_{0}$</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>4.622762836042054e-05</v>
+        <v>4.565585531285447e-05</v>
       </c>
     </row>
     <row r="25">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4.495977211666942e-05</v>
+        <v>4.447190546208865e-05</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4.410302471117616e-05</v>
+        <v>4.379944614525561e-05</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3.993790709861991e-05</v>
+        <v>3.998616213711897e-05</v>
       </c>
     </row>
     <row r="28">
@@ -793,33 +793,33 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>3.987933969575728e-05</v>
+        <v>3.995032543784376e-05</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>(h$_{r}$)$_{2}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3.834908554655299e-05</v>
+        <v>3.852227837479863e-05</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{0}$</t>
+          <t>(h$_{r}$)$_{3}$</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3.816676660348832e-05</v>
+        <v>3.789972913217216e-05</v>
       </c>
     </row>
     <row r="31">
@@ -832,20 +832,20 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>3.711212677301988e-05</v>
+        <v>3.752580069846353e-05</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>(h$_{r}$)$_{3}$</t>
+          <t>(h$_{r}$)$_{2}$</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3.660966904299999e-05</v>
+        <v>3.750724468840098e-05</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3.583060837869911e-05</v>
+        <v>3.597268460202609e-05</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>3.057890512054302e-05</v>
+        <v>3.351675424879212e-05</v>
       </c>
     </row>
     <row r="35">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2.949040729480698e-05</v>
+        <v>2.831506395982808e-05</v>
       </c>
     </row>
     <row r="36">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2.814919362194912e-05</v>
+        <v>2.773139227179528e-05</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2.714584164571424e-05</v>
+        <v>2.7262452011274e-05</v>
       </c>
     </row>
     <row r="38">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2.701444864120941e-05</v>
+        <v>2.695114288782441e-05</v>
       </c>
     </row>
     <row r="39">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2.55883695992144e-05</v>
+        <v>2.643246565534268e-05</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2.246867373782172e-05</v>
+        <v>2.29066411143425e-05</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2.160544375726586e-05</v>
+        <v>2.123584403257723e-05</v>
       </c>
     </row>
     <row r="42">
@@ -975,46 +975,46 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1.950890507889248e-05</v>
+        <v>1.975935653633256e-05</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{0}$</t>
+          <t>(h$_{p}$)$_{1}$</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.894758306539452e-05</v>
+        <v>1.93747513273645e-05</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{1}$</t>
+          <t>$(\eta_{r})_{0}$</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.826489781600642e-05</v>
+        <v>1.849147553331105e-05</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>(h$_{p}$)$_{1}$</t>
+          <t>(h$_{pq}$)$_{1}$</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.791710324174913e-05</v>
+        <v>1.799840081848746e-05</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.704719688083949e-05</v>
+        <v>1.76564529973295e-05</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1.688106423393282e-05</v>
+        <v>1.683009207228131e-05</v>
       </c>
     </row>
     <row r="48">
@@ -1053,46 +1053,46 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.666129833263441e-05</v>
+        <v>1.679797074517646e-05</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
+          <t>$F_{q}$</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.612252912282159e-05</v>
+        <v>1.653591723972108e-05</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>$F_{q}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.604229521877008e-05</v>
+        <v>1.573152552394466e-05</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1.588225473048986e-05</v>
+        <v>1.54443645710913e-05</v>
       </c>
     </row>
     <row r="52">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1.498995365720297e-05</v>
+        <v>1.518898231305793e-05</v>
       </c>
     </row>
     <row r="53">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1.423383538188741e-05</v>
+        <v>1.413317862715608e-05</v>
       </c>
     </row>
     <row r="54">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1.281307617778237e-05</v>
+        <v>1.296527535241432e-05</v>
       </c>
     </row>
     <row r="55">
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1.269429344807427e-05</v>
+        <v>1.247964623404556e-05</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>9.087495543128099e-06</v>
+        <v>9.489814348728603e-06</v>
       </c>
     </row>
     <row r="57">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>8.711569809172401e-06</v>
+        <v>9.009267449402741e-06</v>
       </c>
     </row>
     <row r="58">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>8.081668901448399e-06</v>
+        <v>7.919639178307435e-06</v>
       </c>
     </row>
     <row r="59">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>7.535809050573775e-06</v>
+        <v>7.365645153613365e-06</v>
       </c>
     </row>
     <row r="60">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>6.95451458184978e-06</v>
+        <v>6.898712550157791e-06</v>
       </c>
     </row>
     <row r="61">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>6.951961248364658e-06</v>
+        <v>6.611660775492922e-06</v>
       </c>
     </row>
     <row r="62">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>6.366589623517058e-06</v>
+        <v>6.487266848876169e-06</v>
       </c>
     </row>
     <row r="63">
@@ -1248,7 +1248,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>6.25138880402126e-06</v>
+        <v>6.204787670707869e-06</v>
       </c>
     </row>
     <row r="64">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>6.1269521374055e-06</v>
+        <v>6.093062827095093e-06</v>
       </c>
     </row>
     <row r="65">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>5.668041962610166e-06</v>
+        <v>5.759952306854176e-06</v>
       </c>
     </row>
     <row r="66">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>5.588434477103609e-06</v>
+        <v>5.538180845518032e-06</v>
       </c>
     </row>
     <row r="67">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>4.840742290176363e-06</v>
+        <v>4.877284250885272e-06</v>
       </c>
     </row>
     <row r="68">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4.667352378029287e-06</v>
+        <v>4.525621337882048e-06</v>
       </c>
     </row>
     <row r="69">
@@ -1326,33 +1326,33 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>4.460071073301634e-06</v>
+        <v>4.430655161964942e-06</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>$(F_{p})_{1}$</t>
+          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>4.171753889064693e-06</v>
+        <v>4.225423380743252e-06</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
+          <t>$(F_{p})_{1}$</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>4.112153026927368e-06</v>
+        <v>4.145679804425736e-06</v>
       </c>
     </row>
     <row r="72">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>3.711935004734988e-06</v>
+        <v>3.728544934711371e-06</v>
       </c>
     </row>
     <row r="73">
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>3.627960818214397e-06</v>
+        <v>3.633500390251857e-06</v>
       </c>
     </row>
     <row r="74">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>3.627788469404001e-06</v>
+        <v>3.607939330915683e-06</v>
       </c>
     </row>
     <row r="75">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>3.547691865613434e-06</v>
+        <v>3.446142487066101e-06</v>
       </c>
     </row>
     <row r="76">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>3.001968876133063e-06</v>
+        <v>3.090075014405905e-06</v>
       </c>
     </row>
     <row r="77">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2.36477351018293e-06</v>
+        <v>2.453736191715734e-06</v>
       </c>
     </row>
     <row r="78">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2.328147450586887e-06</v>
+        <v>2.336712420874132e-06</v>
       </c>
     </row>
     <row r="79">
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>2.132721656621876e-06</v>
+        <v>2.029162119557156e-06</v>
       </c>
     </row>
     <row r="80">
@@ -1469,7 +1469,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1.739008240743829e-06</v>
+        <v>1.763645345810022e-06</v>
       </c>
     </row>
     <row r="81">
@@ -1482,33 +1482,33 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1.577513787181985e-06</v>
+        <v>1.528031936514659e-06</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>$(F_{p})_{2}$</t>
+          <t>$(\eta_{p})_{3}$</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1.495265847996235e-06</v>
+        <v>1.490608492816358e-06</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{3}$</t>
+          <t>$(F_{p})_{2}$</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1.426648824721607e-06</v>
+        <v>1.455622467277225e-06</v>
       </c>
     </row>
     <row r="84">
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>7.136711886899882e-07</v>
+        <v>7.030991053320424e-07</v>
       </c>
     </row>
     <row r="85">
@@ -1534,7 +1534,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>3.231686173041558e-07</v>
+        <v>3.034298319814945e-07</v>
       </c>
     </row>
     <row r="86">
@@ -1547,228 +1547,228 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>9.604415461011884e-08</v>
+        <v>9.003849366383107e-08</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>$(F_{p})_{3}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>3.864758805428185e-08</v>
+        <v>4.654496990812673e-08</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>3.491734141652448e-08</v>
+        <v>3.248439725662721e-08</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>$(F_{p})_{3}$</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>3.031815606742942e-08</v>
+        <v>3.181265347291359e-08</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>3.01284612590861e-08</v>
+        <v>2.94778668239382e-08</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$(\omega_{p})_{2}$</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2.537180824221287e-08</v>
+        <v>2.063205841877757e-08</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{1}$</t>
+          <t>$(\omega_{r})_{1}$</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2.091661457573565e-08</v>
+        <v>2.057912345873382e-08</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{1}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1.601743786452314e-08</v>
+        <v>2.037538446634959e-08</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{3}$</t>
+          <t>type_0</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1.597354860012317e-08</v>
+        <v>1.477521927925031e-08</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{2}$</t>
+          <t>(h$_{rs}$)$_{0}$</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1.390480466866094e-08</v>
+        <v>1.454319361954811e-08</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>(h$_{rs}$)$_{0}$</t>
+          <t>$(\omega_{r})_{0}$</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1.19028862607047e-08</v>
+        <v>1.265740218356881e-08</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{0}$</t>
+          <t>$(\omega_{r})_{3}$</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1.1446987565978e-08</v>
+        <v>1.244621199806713e-08</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>type_0</t>
+          <t>$\mathbf{b}$</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1.121630698655168e-08</v>
+        <v>8.700893674223822e-09</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>$\omega_{s}$</t>
+          <t>$(\omega_{p})_{1}$</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>5.283961517545795e-09</v>
+        <v>5.005227185111558e-09</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>$\mathbf{b}$</t>
+          <t>$\omega_{q}$</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>1.05105372227303e-09</v>
+        <v>3.500057336255808e-09</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>$\omega_{q}$</t>
+          <t>$\omega_{s}$</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8.179965055297305e-10</v>
+        <v>2.639809626868773e-09</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>$\eta_{q}$</t>
+          <t>$(\omega_{p})_{3}$</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>4.556955910722854e-10</v>
+        <v>1.644199942163898e-09</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{3}$</t>
+          <t>$\eta_{q}$</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1.418092216990453e-10</v>
+        <v>4.317328074389671e-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tue Feb  4 10:18:33 AM EST 2025
</commit_message>
<xml_diff>
--- a/ozone/ozone_MB_SHAP.xlsx
+++ b/ozone/ozone_MB_SHAP.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0008892552225074907</v>
+        <v>0.0008939121986040734</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0006776076343631585</v>
+        <v>0.0006749952681096833</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0004218182197812181</v>
+        <v>0.000417295443565566</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.0003765456554795044</v>
+        <v>0.0003780690076164485</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.0003169586951895845</v>
+        <v>0.0003190170992704266</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.0002821837277648635</v>
+        <v>0.000290456345059997</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.000263599993350192</v>
+        <v>0.0002642698241043285</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.0001779199314815862</v>
+        <v>0.000178032412925192</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.0001618232092465177</v>
+        <v>0.0001610359535311469</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.0001172200347640319</v>
+        <v>0.0001198143315554234</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.0001161616065326009</v>
+        <v>0.0001141978222358567</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.0001061750901893721</v>
+        <v>0.0001029718203552676</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9.137179801422224e-05</v>
+        <v>8.983421693672707e-05</v>
       </c>
     </row>
     <row r="15">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8.436900978575903e-05</v>
+        <v>8.477129753548767e-05</v>
       </c>
     </row>
     <row r="16">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>7.760257865862746e-05</v>
+        <v>7.814359288473629e-05</v>
       </c>
     </row>
     <row r="17">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6.665416177921328e-05</v>
+        <v>6.833080695786403e-05</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>6.609285404120526e-05</v>
+        <v>6.689694169855833e-05</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>6.224987514591092e-05</v>
+        <v>6.153987659244439e-05</v>
       </c>
     </row>
     <row r="20">
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6.142815711096499e-05</v>
+        <v>6.09994325209579e-05</v>
       </c>
     </row>
     <row r="21">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6.031932114596838e-05</v>
+        <v>6.031290888366295e-05</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>4.931637474349794e-05</v>
+        <v>4.939792260511538e-05</v>
       </c>
     </row>
     <row r="23">
@@ -728,33 +728,33 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4.677905199246879e-05</v>
+        <v>4.65261629682723e-05</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>(h$_{pq}$)$_{2}$</t>
+          <t>(h$_{pr}$)$_{3}$</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>4.476402805394986e-05</v>
+        <v>4.502228883294549e-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>(h$_{pr}$)$_{3}$</t>
+          <t>(h$_{pq}$)$_{2}$</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4.441662147270612e-05</v>
+        <v>4.467880786697934e-05</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4.392259925439911e-05</v>
+        <v>4.342032329911382e-05</v>
       </c>
     </row>
     <row r="27">
@@ -780,33 +780,33 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4.008315689715553e-05</v>
+        <v>4.000277612047268e-05</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>(h$_{r}$)$_{2}$</t>
+          <t>$F_{s}$</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>3.841096886392836e-05</v>
+        <v>3.959587678930198e-05</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>$F_{s}$</t>
+          <t>(h$_{r}$)$_{2}$</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3.832646188662629e-05</v>
+        <v>3.834311846226618e-05</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3.819268052465107e-05</v>
+        <v>3.794023953174323e-05</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>3.761096707621735e-05</v>
+        <v>3.792331513884148e-05</v>
       </c>
     </row>
     <row r="32">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3.741159163336254e-05</v>
+        <v>3.775333273441231e-05</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3.595038121173624e-05</v>
+        <v>3.539565223401197e-05</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>3.156820229723709e-05</v>
+        <v>3.193173444407881e-05</v>
       </c>
     </row>
     <row r="35">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>2.953522764720236e-05</v>
+        <v>2.962519600775321e-05</v>
       </c>
     </row>
     <row r="36">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>2.77964945386009e-05</v>
+        <v>2.773982478672589e-05</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>2.739399323035937e-05</v>
+        <v>2.758421325778318e-05</v>
       </c>
     </row>
     <row r="38">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2.680716682388106e-05</v>
+        <v>2.742261031145537e-05</v>
       </c>
     </row>
     <row r="39">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>2.674649015766396e-05</v>
+        <v>2.688817442583975e-05</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>2.285409473116895e-05</v>
+        <v>2.300130577309239e-05</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2.149879209193023e-05</v>
+        <v>2.165383058631292e-05</v>
       </c>
     </row>
     <row r="42">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>2.002463973982095e-05</v>
+        <v>1.992503167789412e-05</v>
       </c>
     </row>
     <row r="43">
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.866916359273385e-05</v>
+        <v>1.965957284425124e-05</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.838759804174708e-05</v>
+        <v>1.846661532542195e-05</v>
       </c>
     </row>
     <row r="45">
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1.823433243068136e-05</v>
+        <v>1.800917038278286e-05</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1.78590309526702e-05</v>
+        <v>1.780613357076488e-05</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1.716108678482271e-05</v>
+        <v>1.695633875209248e-05</v>
       </c>
     </row>
     <row r="48">
@@ -1053,46 +1053,46 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1.678683957782912e-05</v>
+        <v>1.653265493906129e-05</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
+          <t>$F_{q}$</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.616334270595508e-05</v>
+        <v>1.608993773054081e-05</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>$F_{q}$</t>
+          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1.614763434417835e-05</v>
+        <v>1.588524886995224e-05</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>$(\langle rr \vert rr \rangle)_{2}$</t>
+          <t>$(\langle pq \vert rs \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1.570083041490085e-05</v>
+        <v>1.577990099527796e-05</v>
       </c>
     </row>
     <row r="52">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1.508925831411055e-05</v>
+        <v>1.487376350715456e-05</v>
       </c>
     </row>
     <row r="53">
@@ -1118,33 +1118,33 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1.424880483408442e-05</v>
+        <v>1.425215336092793e-05</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>$\eta_{s}$</t>
+          <t>$(\omega_{p})_{0}$</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1.290858371315934e-05</v>
+        <v>1.25749973060615e-05</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{0}$</t>
+          <t>$\eta_{s}$</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1.2708536102171e-05</v>
+        <v>1.219210023417441e-05</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>9.205525756419943e-06</v>
+        <v>9.400822314449698e-06</v>
       </c>
     </row>
     <row r="57">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>9.081527878458481e-06</v>
+        <v>8.83672459988667e-06</v>
       </c>
     </row>
     <row r="58">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>8.051452999969116e-06</v>
+        <v>8.002184029049534e-06</v>
       </c>
     </row>
     <row r="59">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>7.358086587503526e-06</v>
+        <v>7.773497116770327e-06</v>
       </c>
     </row>
     <row r="60">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>7.088282423278895e-06</v>
+        <v>6.934287438516747e-06</v>
       </c>
     </row>
     <row r="61">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>6.868971842904003e-06</v>
+        <v>6.707737890902148e-06</v>
       </c>
     </row>
     <row r="62">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>6.489261489953045e-06</v>
+        <v>6.515665493591137e-06</v>
       </c>
     </row>
     <row r="63">
@@ -1248,7 +1248,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>6.318327670216003e-06</v>
+        <v>6.37992839657438e-06</v>
       </c>
     </row>
     <row r="64">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>6.188044321321396e-06</v>
+        <v>6.323176553834863e-06</v>
       </c>
     </row>
     <row r="65">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>5.772977922155292e-06</v>
+        <v>5.763640820931741e-06</v>
       </c>
     </row>
     <row r="66">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>5.525014456901111e-06</v>
+        <v>5.530928990260214e-06</v>
       </c>
     </row>
     <row r="67">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>4.81477978637754e-06</v>
+        <v>4.867065064817177e-06</v>
       </c>
     </row>
     <row r="68">
@@ -1313,72 +1313,72 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>4.534229846952481e-06</v>
+        <v>4.478877549390703e-06</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>$(F_{p})_{1}$</t>
+          <t>$type_2$</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>4.276711829751058e-06</v>
+        <v>4.406606867648321e-06</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
+          <t>$(F_{p})_{1}$</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>4.224029367340138e-06</v>
+        <v>4.356473673685131e-06</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>$type_2$</t>
+          <t>$(F_{r}^{\text{SCF}})_{3}$</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>4.20460347654053e-06</v>
+        <v>4.109587831762429e-06</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
+          <t>$(\eta_{r})_{2}$</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>3.74999930200561e-06</v>
+        <v>3.719487912802046e-06</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>$(\eta_{r})_{2}$</t>
+          <t>$(\langle pp \vert pp \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>3.638890135239479e-06</v>
+        <v>3.67550498013907e-06</v>
       </c>
     </row>
     <row r="74">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>3.629073264711836e-06</v>
+        <v>3.543625495980721e-06</v>
       </c>
     </row>
     <row r="75">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>3.510968442180456e-06</v>
+        <v>3.416834637590532e-06</v>
       </c>
     </row>
     <row r="76">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>2.92596904327747e-06</v>
+        <v>3.063879636861552e-06</v>
       </c>
     </row>
     <row r="77">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2.460464617639222e-06</v>
+        <v>2.508079065744602e-06</v>
       </c>
     </row>
     <row r="78">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>2.369091502793501e-06</v>
+        <v>2.253575967651358e-06</v>
       </c>
     </row>
     <row r="79">
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>2.102365614181298e-06</v>
+        <v>2.114986125894094e-06</v>
       </c>
     </row>
     <row r="80">
@@ -1469,46 +1469,46 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1.77474324129859e-06</v>
+        <v>1.739407909806053e-06</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>$(F_{p})_{2}$</t>
+          <t>$(\eta_{p})_{3}$</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1.534202945859339e-06</v>
+        <v>1.551937754210229e-06</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{2}$</t>
+          <t>$(F_{p})_{2}$</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1.506347614586752e-06</v>
+        <v>1.51437599437738e-06</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>$(\eta_{p})_{3}$</t>
+          <t>$(\eta_{p})_{2}$</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1.370469353465881e-06</v>
+        <v>1.505936629599036e-06</v>
       </c>
     </row>
     <row r="84">
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>7.4131753828976e-07</v>
+        <v>7.186594433268784e-07</v>
       </c>
     </row>
     <row r="85">
@@ -1534,7 +1534,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>2.886832032721551e-07</v>
+        <v>3.209896098325893e-07</v>
       </c>
     </row>
     <row r="86">
@@ -1547,59 +1547,59 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>8.471288768267502e-08</v>
+        <v>7.796484509038682e-08</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>3.024944627609659e-08</v>
+        <v>6.482310261648045e-08</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>$(F_{p})_{3}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{3}$</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>2.897218793969686e-08</v>
+        <v>4.875354434503296e-08</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>$type_0$</t>
+          <t>$(F_{p})_{3}$</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>2.806609936770687e-08</v>
+        <v>3.127032260511813e-08</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2.718529393792282e-08</v>
+        <v>2.650666839959123e-08</v>
       </c>
     </row>
     <row r="91">
@@ -1612,137 +1612,137 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>2.129332987139472e-08</v>
+        <v>2.105066786859708e-08</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{1}$</t>
+          <t>$(\omega_{p})_{2}$</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>2.08494733057455e-08</v>
+        <v>1.902253489822108e-08</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{1}$</t>
+          <t>$type_0$</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1.967055429854626e-08</v>
+        <v>1.819566422397973e-08</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>$(\langle pq \vert sr \rangle)_{2}$</t>
+          <t>$(\omega_{r})_{3}$</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1.925970954975286e-08</v>
+        <v>1.808518129591661e-08</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{3}$</t>
+          <t>$(\langle pq \vert sr \rangle)_{0}$</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1.892729815990517e-08</v>
+        <v>1.669330046559723e-08</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>$\omega_{s}$</t>
+          <t>(h$_{rs}$)$_{0}$</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1.815645642307919e-08</v>
+        <v>8.459537605023353e-09</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>$(\omega_{r})_{1}$</t>
+          <t>$\omega_{s}$</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1.484958757914115e-08</v>
+        <v>7.413743962668076e-09</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>$(\omega_{p})_{2}$</t>
+          <t>$(\omega_{p})_{1}$</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>1.20669038860983e-08</v>
+        <v>4.383706751824972e-09</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>(h$_{rs}$)$_{0}$</t>
+          <t>$(\omega_{r})_{1}$</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1.089875441951313e-08</v>
+        <v>3.656948125825397e-09</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>$\eta_{q}$</t>
+          <t>$\mathbf{b}$</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>3.400179300333807e-09</v>
+        <v>3.462539316647511e-09</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>$\mathbf{b}$</t>
+          <t>$\eta_{q}$</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>2.685787764750484e-09</v>
+        <v>3.165242136945541e-09</v>
       </c>
     </row>
     <row r="102">
@@ -1755,7 +1755,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>1.61497801443314e-09</v>
+        <v>8.609154523189484e-10</v>
       </c>
     </row>
     <row r="103">
@@ -1768,7 +1768,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>4.090690866067805e-10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>